<commit_message>
can execute HSA with reduced landmarks
</commit_message>
<xml_diff>
--- a/franz_hsa/hsa_calculation/hsa_execution_parameters.xlsx
+++ b/franz_hsa/hsa_calculation/hsa_execution_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\hsa_calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F11168-A231-4ED9-94C9-BFCFB2823A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51082423-99B4-49ED-A8C9-002D6B0732C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>data_type</t>
   </si>
@@ -60,9 +60,6 @@
     <t>landmark_placement</t>
   </si>
   <si>
-    <t>manual</t>
-  </si>
-  <si>
     <t>export_landmarks</t>
   </si>
   <si>
@@ -76,6 +73,12 @@
   </si>
   <si>
     <t>exp_data_path</t>
+  </si>
+  <si>
+    <t>manually</t>
+  </si>
+  <si>
+    <t>verbose</t>
   </si>
 </sst>
 </file>
@@ -134,10 +137,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,9 +445,9 @@
     <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -454,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -472,13 +477,16 @@
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -486,13 +494,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="2">
         <v>200</v>
@@ -507,12 +515,15 @@
         <v>0</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="L2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" s="4" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made an ID for Tareq
</commit_message>
<xml_diff>
--- a/franz_hsa/hsa_calculation/hsa_execution_parameters.xlsx
+++ b/franz_hsa/hsa_calculation/hsa_execution_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\hsa_calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A0BD2D-FF54-4AB8-B4F8-F54E3C6383D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABED933-661D-4B9B-8EA9-12E76598F988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>data_type</t>
   </si>
@@ -448,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,6 +660,50 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>200</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>